<commit_message>
finish acceptance test plan
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yatlo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\ychan\swen-261\lowercase_h\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BE8999-38D3-43A6-8ACD-D8FDEB1E676D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769C9E6B-8717-44CE-A124-9268E32778A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>User Story</t>
   </si>
@@ -545,12 +545,78 @@
   <si>
     <t>Given I CORRECTLY ENTER THE ADMIN USERNAME when I LOG IN then I SHOULD HAVE ACCESS TO THE MANAGER.</t>
   </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>As a Manager I want to manage my needs so that helpers will fund them.</t>
+  </si>
+  <si>
+    <t>Given I am logged in as admin when I am on the cupboard page then I expect to see a means to add a new need.</t>
+  </si>
+  <si>
+    <t>Given I am logged in as admin when I add a new need then I expect to see that need in the cupboard.</t>
+  </si>
+  <si>
+    <t>Given I am logged in as admin when I click on a delete need button then I expect the need to be removed from the cupboard.</t>
+  </si>
+  <si>
+    <t>Given I am on a need's detail page when I edit the need then the system should update the need for the future.</t>
+  </si>
+  <si>
+    <t>Given I am logged in when I am on the homepage then I expect to see a means to search.</t>
+  </si>
+  <si>
+    <t>Given I am logged in when I type into the search bar then I expect to see results for individual needs.</t>
+  </si>
+  <si>
+    <t>BH;03/18/2024</t>
+  </si>
+  <si>
+    <t>GO;03/18/2024</t>
+  </si>
+  <si>
+    <t>As a helper I want to checkout my funding basket so that I can contribute to my selected needs.</t>
+  </si>
+  <si>
+    <t>Given that I am on my funding basket page when I reach the end of my funding basket then I expect to see a means to checkout.</t>
+  </si>
+  <si>
+    <t>Given that I am on the confirmation page when I click the confirm the checkout then I expect my contributions to be made towards the needs in my basket and navigate back to the homepage.</t>
+  </si>
+  <si>
+    <t>Given that my funding basket is not empty when I click the checkout button then I expect to be taken to the confirmation page.</t>
+  </si>
+  <si>
+    <t>AS a Developer I WANT to create a PASSWORD I can access the HELPER PAGE MORE SECURELY</t>
+  </si>
+  <si>
+    <t>Given I HAVE INPUT THE RIGHT PASSWORD when LOG IN WITH A USERNAME AND PASSWORD then I SHOULD GO TO THE HELPER PAGE</t>
+  </si>
+  <si>
+    <t>Given I HAVE INPUT A UNIQUE PASSWORD AND USERNAME when SIGN IN then A NEW USER SHOULD BE CREATED</t>
+  </si>
+  <si>
+    <t>AS a User I WANT a BETTER UI  SO THAT I can access the SITE WITH MORE EASE.</t>
+  </si>
+  <si>
+    <t>Given THE SITE IS ACTIVE when I USE THE SITE then I EXPECT THE SITE TO HAVE GOOD VISUALS AND UI.</t>
+  </si>
+  <si>
+    <t>AS a User I WANT to solve riddles SO THAT I can access my page more securely.</t>
+  </si>
+  <si>
+    <t>Given I HAVE INPUT THE RIGHT ANSWER when LOG IN WITH A USERNAME, RIDDLE, AND PASSWORD then I SHOULD GO TO MY HOMEPAGE</t>
+  </si>
+  <si>
+    <t>Given I am not logged in when I am on a login page then I should be given a random riddle to solve.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,16 +686,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -653,11 +740,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -687,6 +794,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1042,9 +1161,9 @@
   </sheetPr>
   <dimension ref="A1:F587"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1077,176 +1196,301 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E4" s="5"/>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="45.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="5"/>
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="63.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="5"/>
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="5"/>
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="5"/>
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="5"/>
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="5"/>
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="1" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="C18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="C19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13" t="s">
+        <v>39</v>
+      </c>
       <c r="C21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" s="1" customFormat="1" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="C22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" s="1" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="C23" s="5"/>
       <c r="E23" s="5"/>
     </row>
-    <row r="24" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="C24" s="5"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="5"/>
       <c r="E25" s="5"/>
     </row>
-    <row r="26" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="5"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="5"/>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="5"/>
       <c r="E29" s="5"/>
     </row>
-    <row r="30" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C30" s="5"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="3:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="3:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="5"/>
       <c r="E32" s="5"/>
     </row>

</xml_diff>